<commit_message>
need discusion and conclusion
</commit_message>
<xml_diff>
--- a/data process.xlsx
+++ b/data process.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Impact velocity</t>
   </si>
@@ -31,6 +31,33 @@
   </si>
   <si>
     <t>core thickness</t>
+  </si>
+  <si>
+    <t>Sensitive Analyse</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>mesh convergence</t>
+  </si>
+  <si>
+    <t>velosity</t>
+  </si>
+  <si>
+    <t>Core thickness</t>
+  </si>
+  <si>
+    <t>Ballistic Limit</t>
+  </si>
+  <si>
+    <t>60 m/s</t>
+  </si>
+  <si>
+    <t>font face</t>
+  </si>
+  <si>
+    <t>Thickness of Front Face-sheet</t>
   </si>
 </sst>
 </file>
@@ -54,10 +81,36 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -66,11 +119,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -106,10 +164,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12026843949895484"/>
-          <c:y val="0.15160476752642452"/>
-          <c:w val="0.82489467259706306"/>
-          <c:h val="0.68305028853519667"/>
+          <c:x val="0.134390099047838"/>
+          <c:y val="0.17838913825345989"/>
+          <c:w val="0.79185776960361698"/>
+          <c:h val="0.64217058755138956"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -165,9 +223,6 @@
                 <c:pt idx="10">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>700</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -209,9 +264,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -226,11 +278,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92385280"/>
-        <c:axId val="92386816"/>
+        <c:axId val="213244544"/>
+        <c:axId val="213250432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92385280"/>
+        <c:axId val="213244544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -240,12 +292,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92386816"/>
+        <c:crossAx val="213250432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92386816"/>
+        <c:axId val="213250432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -256,7 +308,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92385280"/>
+        <c:crossAx val="213244544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -267,10 +319,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.71484124968249929"/>
-          <c:y val="0.73025096023720015"/>
-          <c:w val="0.17145097790195579"/>
-          <c:h val="7.6663081425043411E-2"/>
+          <c:x val="0.72037454259823364"/>
+          <c:y val="0.75004145470763472"/>
+          <c:w val="0.15518193673619876"/>
+          <c:h val="7.0601874268512346E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -309,9 +361,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.12574269000321125"/>
-          <c:y val="0.14090546988335723"/>
-          <c:w val="0.81307402463252521"/>
-          <c:h val="0.67496129021608153"/>
+          <c:y val="0.14090562816965485"/>
+          <c:w val="0.82465597872372221"/>
+          <c:h val="0.68315392140438691"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -321,15 +373,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Impact velocity</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Simulation</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -404,14 +448,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="102650624"/>
-        <c:axId val="102652544"/>
+        <c:axId val="215977984"/>
+        <c:axId val="215979904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102650624"/>
+        <c:axId val="215977984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="800"/>
+          <c:max val="700"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -439,15 +483,15 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102652544"/>
+        <c:crossAx val="215979904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102652544"/>
+        <c:axId val="215979904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="600"/>
+          <c:max val="450"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -480,7 +524,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102650624"/>
+        <c:crossAx val="215977984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -501,8 +545,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.67943815767062987"/>
-          <c:y val="0.62543567038145786"/>
+          <c:x val="0.68955838774422651"/>
+          <c:y val="0.66247280954187826"/>
           <c:w val="0.24061635766004211"/>
           <c:h val="7.5819343336799877E-2"/>
         </c:manualLayout>
@@ -617,11 +661,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="102676736"/>
-        <c:axId val="102687104"/>
+        <c:axId val="216418176"/>
+        <c:axId val="216420352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102676736"/>
+        <c:axId val="216418176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20000"/>
@@ -652,12 +696,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102687104"/>
+        <c:crossAx val="216420352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102687104"/>
+        <c:axId val="216420352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -689,7 +733,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102676736"/>
+        <c:crossAx val="216418176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -811,11 +855,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="104486400"/>
-        <c:axId val="104488320"/>
+        <c:axId val="216450176"/>
+        <c:axId val="216452096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104486400"/>
+        <c:axId val="216450176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -844,12 +888,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104488320"/>
+        <c:crossAx val="216452096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104488320"/>
+        <c:axId val="216452096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +928,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104486400"/>
+        <c:crossAx val="216450176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -931,22 +975,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5690</c:v>
+                  <c:v>9655</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8840</c:v>
+                  <c:v>13796</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11231</c:v>
+                  <c:v>17382</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22580</c:v>
+                  <c:v>19634</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30560</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>40281</c:v>
+                  <c:v>24352</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,22 +999,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>220</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>194</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>192</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>191</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>190</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -988,11 +1026,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="104496512"/>
-        <c:axId val="104519168"/>
+        <c:axId val="216464384"/>
+        <c:axId val="216487040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104496512"/>
+        <c:axId val="216464384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,12 +1059,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104519168"/>
+        <c:crossAx val="216487040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104519168"/>
+        <c:axId val="216487040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,7 +1094,298 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104496512"/>
+        <c:crossAx val="216464384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$52:$Q$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$52:$R$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="188271616"/>
+        <c:axId val="188270080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="188271616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188270080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="188270080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188271616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$64:$A$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$64:$B$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="202412416"/>
+        <c:axId val="202410624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="202412416"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="30"/>
+          <c:min val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Core Thickness (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="202410624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="202410624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="65"/>
+          <c:min val="40"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Ballistic Limit (m/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="202412416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1077,16 +1406,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>100011</xdr:rowOff>
+      <xdr:rowOff>100010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1108,15 +1437,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1220,6 +1549,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1515,15 +1904,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:X78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1693,14 +2082,6 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>700</v>
-      </c>
-      <c r="B27">
-        <v>550</v>
-      </c>
-    </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P31" t="s">
         <v>3</v>
@@ -1717,10 +2098,10 @@
         <v>1</v>
       </c>
       <c r="P32">
-        <v>5690</v>
+        <v>9655</v>
       </c>
       <c r="Q32">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -1731,10 +2112,10 @@
         <v>220</v>
       </c>
       <c r="P33">
-        <v>8840</v>
+        <v>13796</v>
       </c>
       <c r="Q33">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -1745,10 +2126,10 @@
         <v>155</v>
       </c>
       <c r="P34">
-        <v>11231</v>
+        <v>17382</v>
       </c>
       <c r="Q34">
-        <v>194</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -1759,10 +2140,10 @@
         <v>145</v>
       </c>
       <c r="P35">
-        <v>22580</v>
+        <v>19634</v>
       </c>
       <c r="Q35">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -1773,10 +2154,10 @@
         <v>142</v>
       </c>
       <c r="P36">
-        <v>30560</v>
+        <v>24352</v>
       </c>
       <c r="Q36">
-        <v>191</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -1786,12 +2167,6 @@
       <c r="B37">
         <v>140</v>
       </c>
-      <c r="P37">
-        <v>40281</v>
-      </c>
-      <c r="Q37">
-        <v>190</v>
-      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1809,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>25</v>
       </c>
@@ -1817,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>20</v>
       </c>
@@ -1825,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -1833,31 +2208,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>12</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q52">
+        <v>300</v>
+      </c>
+      <c r="R52">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>10</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q53">
+        <v>100</v>
+      </c>
+      <c r="R53">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>8</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q54">
+        <v>80</v>
+      </c>
+      <c r="R54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>5</v>
       </c>
@@ -1865,7 +2258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2</v>
       </c>
@@ -1873,9 +2266,214 @@
         <v>15</v>
       </c>
     </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" t="s">
+        <v>8</v>
+      </c>
+      <c r="I62">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" t="s">
+        <v>3</v>
+      </c>
+      <c r="H63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>13796</v>
+      </c>
+      <c r="H64">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>30</v>
+      </c>
+      <c r="B65">
+        <v>60</v>
+      </c>
+      <c r="F65">
+        <v>17382</v>
+      </c>
+      <c r="H65">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>20</v>
+      </c>
+      <c r="B66">
+        <v>58</v>
+      </c>
+      <c r="F66">
+        <v>19634</v>
+      </c>
+      <c r="H66">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>15</v>
+      </c>
+      <c r="B67">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>10</v>
+      </c>
+      <c r="B68">
+        <v>56</v>
+      </c>
+      <c r="S68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T68" s="1"/>
+      <c r="W68" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="X68" s="2"/>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>56</v>
+      </c>
+      <c r="S69">
+        <v>25</v>
+      </c>
+      <c r="T69">
+        <v>19.8</v>
+      </c>
+      <c r="U69">
+        <v>10</v>
+      </c>
+      <c r="W69" s="3">
+        <v>3</v>
+      </c>
+      <c r="X69" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S70">
+        <v>5</v>
+      </c>
+      <c r="T70">
+        <v>21.6</v>
+      </c>
+      <c r="U70">
+        <v>7</v>
+      </c>
+      <c r="W70" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="X70" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W71" s="3">
+        <v>2</v>
+      </c>
+      <c r="X71" s="3"/>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="W72" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="X72" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>3</v>
+      </c>
+      <c r="B73">
+        <v>60</v>
+      </c>
+      <c r="W73" s="3"/>
+      <c r="X73" s="3"/>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2.5</v>
+      </c>
+      <c r="B74">
+        <v>56</v>
+      </c>
+      <c r="W74" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1.5</v>
+      </c>
+      <c r="B76">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="S68:T68"/>
+    <mergeCell ref="W68:X68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>